<commit_message>
change in db location and name
</commit_message>
<xml_diff>
--- a/data/minutes/copom_dates.xlsx
+++ b/data/minutes/copom_dates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="9">
   <si>
     <t>date</t>
   </si>
@@ -38,6 +38,9 @@
   </si>
   <si>
     <t>Roberto Campos Neto</t>
+  </si>
+  <si>
+    <t>decision_date</t>
   </si>
 </sst>
 </file>
@@ -380,19 +383,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C210"/>
+  <dimension ref="A1:J210"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I5" sqref="I5:J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -402,8 +407,11 @@
       <c r="C1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>36560</v>
       </c>
@@ -413,8 +421,12 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <f>A2-8</f>
+        <v>36552</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>36571</v>
       </c>
@@ -424,8 +436,12 @@
       <c r="C3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D66" si="0">A3-8</f>
+        <v>36563</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>36615</v>
       </c>
@@ -435,8 +451,12 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>36607</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>36650</v>
       </c>
@@ -446,8 +466,14 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>36642</v>
+      </c>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>36686</v>
       </c>
@@ -457,8 +483,12 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>36678</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>36713</v>
       </c>
@@ -468,8 +498,12 @@
       <c r="C7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>36705</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>36739</v>
       </c>
@@ -479,8 +513,12 @@
       <c r="C8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>36731</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>36781</v>
       </c>
@@ -490,8 +528,12 @@
       <c r="C9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>36773</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>36803</v>
       </c>
@@ -501,8 +543,12 @@
       <c r="C10" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>36795</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>36831</v>
       </c>
@@ -512,8 +558,12 @@
       <c r="C11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="1">
+        <f t="shared" si="0"/>
+        <v>36823</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>36867</v>
       </c>
@@ -523,8 +573,12 @@
       <c r="C12" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D12" s="1">
+        <f t="shared" si="0"/>
+        <v>36859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>36901</v>
       </c>
@@ -534,8 +588,12 @@
       <c r="C13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D13" s="1">
+        <f t="shared" si="0"/>
+        <v>36893</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>36943</v>
       </c>
@@ -545,8 +603,12 @@
       <c r="C14" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="1">
+        <f t="shared" si="0"/>
+        <v>36935</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>36978</v>
       </c>
@@ -556,8 +618,12 @@
       <c r="C15" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="1">
+        <f t="shared" si="0"/>
+        <v>36970</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>36979</v>
       </c>
@@ -567,8 +633,12 @@
       <c r="C16" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D16" s="1">
+        <f t="shared" si="0"/>
+        <v>36971</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>37008</v>
       </c>
@@ -578,8 +648,12 @@
       <c r="C17" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="1">
+        <f t="shared" si="0"/>
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>37043</v>
       </c>
@@ -589,8 +663,12 @@
       <c r="C18" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" s="1">
+        <f t="shared" si="0"/>
+        <v>37035</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>37075</v>
       </c>
@@ -600,8 +678,12 @@
       <c r="C19" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" s="1">
+        <f t="shared" si="0"/>
+        <v>37067</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>37102</v>
       </c>
@@ -611,8 +693,12 @@
       <c r="C20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" s="1">
+        <f t="shared" si="0"/>
+        <v>37094</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>37137</v>
       </c>
@@ -622,8 +708,12 @@
       <c r="C21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="1">
+        <f t="shared" si="0"/>
+        <v>37129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>37162</v>
       </c>
@@ -633,8 +723,12 @@
       <c r="C22" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D22" s="1">
+        <f t="shared" si="0"/>
+        <v>37154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>37194</v>
       </c>
@@ -644,8 +738,12 @@
       <c r="C23" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D23" s="1">
+        <f t="shared" si="0"/>
+        <v>37186</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>37228</v>
       </c>
@@ -655,8 +753,12 @@
       <c r="C24" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D24" s="1">
+        <f t="shared" si="0"/>
+        <v>37220</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>37259</v>
       </c>
@@ -666,8 +768,12 @@
       <c r="C25" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D25" s="1">
+        <f t="shared" si="0"/>
+        <v>37251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>37291</v>
       </c>
@@ -677,8 +783,12 @@
       <c r="C26" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D26" s="1">
+        <f t="shared" si="0"/>
+        <v>37283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>37319</v>
       </c>
@@ -688,8 +798,12 @@
       <c r="C27" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D27" s="1">
+        <f t="shared" si="0"/>
+        <v>37311</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>37347</v>
       </c>
@@ -699,8 +813,12 @@
       <c r="C28" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D28" s="1">
+        <f t="shared" si="0"/>
+        <v>37339</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>37375</v>
       </c>
@@ -710,8 +828,12 @@
       <c r="C29" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D29" s="1">
+        <f t="shared" si="0"/>
+        <v>37367</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>37410</v>
       </c>
@@ -721,8 +843,12 @@
       <c r="C30" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D30" s="1">
+        <f t="shared" si="0"/>
+        <v>37402</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>37435</v>
       </c>
@@ -732,8 +858,12 @@
       <c r="C31" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D31" s="1">
+        <f t="shared" si="0"/>
+        <v>37427</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>37464</v>
       </c>
@@ -743,8 +873,12 @@
       <c r="C32" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D32" s="1">
+        <f t="shared" si="0"/>
+        <v>37456</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>37498</v>
       </c>
@@ -754,8 +888,12 @@
       <c r="C33" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" s="1">
+        <f t="shared" si="0"/>
+        <v>37490</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>37526</v>
       </c>
@@ -765,8 +903,12 @@
       <c r="C34" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D34" s="1">
+        <f t="shared" si="0"/>
+        <v>37518</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>37547</v>
       </c>
@@ -776,8 +918,12 @@
       <c r="C35" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
+        <v>37539</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>37560</v>
       </c>
@@ -787,8 +933,12 @@
       <c r="C36" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D36" s="1">
+        <f t="shared" si="0"/>
+        <v>37552</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>37589</v>
       </c>
@@ -798,8 +948,12 @@
       <c r="C37" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D37" s="1">
+        <f t="shared" si="0"/>
+        <v>37581</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37617</v>
       </c>
@@ -809,8 +963,12 @@
       <c r="C38" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D38" s="1">
+        <f t="shared" si="0"/>
+        <v>37609</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37651</v>
       </c>
@@ -820,8 +978,12 @@
       <c r="C39" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D39" s="1">
+        <f t="shared" si="0"/>
+        <v>37643</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>37678</v>
       </c>
@@ -831,8 +993,12 @@
       <c r="C40" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D40" s="1">
+        <f t="shared" si="0"/>
+        <v>37670</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>37707</v>
       </c>
@@ -842,8 +1008,12 @@
       <c r="C41" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D41" s="1">
+        <f t="shared" si="0"/>
+        <v>37699</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>37741</v>
       </c>
@@ -853,8 +1023,12 @@
       <c r="C42" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D42" s="1">
+        <f t="shared" si="0"/>
+        <v>37733</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>37771</v>
       </c>
@@ -864,8 +1038,12 @@
       <c r="C43" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D43" s="1">
+        <f t="shared" si="0"/>
+        <v>37763</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>37799</v>
       </c>
@@ -875,8 +1053,12 @@
       <c r="C44" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D44" s="1">
+        <f t="shared" si="0"/>
+        <v>37791</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>37833</v>
       </c>
@@ -886,8 +1068,12 @@
       <c r="C45" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D45" s="1">
+        <f t="shared" si="0"/>
+        <v>37825</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>37862</v>
       </c>
@@ -897,8 +1083,12 @@
       <c r="C46" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D46" s="1">
+        <f t="shared" si="0"/>
+        <v>37854</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>37889</v>
       </c>
@@ -908,8 +1098,12 @@
       <c r="C47" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D47" s="1">
+        <f t="shared" si="0"/>
+        <v>37881</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>37925</v>
       </c>
@@ -919,8 +1113,12 @@
       <c r="C48" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48" s="1">
+        <f t="shared" si="0"/>
+        <v>37917</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>37953</v>
       </c>
@@ -930,8 +1128,12 @@
       <c r="C49" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49" s="1">
+        <f t="shared" si="0"/>
+        <v>37945</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>37979</v>
       </c>
@@ -941,8 +1143,12 @@
       <c r="C50" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50" s="1">
+        <f t="shared" si="0"/>
+        <v>37971</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>38016</v>
       </c>
@@ -952,8 +1158,12 @@
       <c r="C51" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" s="1">
+        <f t="shared" si="0"/>
+        <v>38008</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>38044</v>
       </c>
@@ -963,8 +1173,12 @@
       <c r="C52" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D52" s="1">
+        <f t="shared" si="0"/>
+        <v>38036</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>38076</v>
       </c>
@@ -974,8 +1188,12 @@
       <c r="C53" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D53" s="1">
+        <f t="shared" si="0"/>
+        <v>38068</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>38103</v>
       </c>
@@ -985,8 +1203,12 @@
       <c r="C54" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D54" s="1">
+        <f t="shared" si="0"/>
+        <v>38095</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>38135</v>
       </c>
@@ -996,8 +1218,12 @@
       <c r="C55" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D55" s="1">
+        <f t="shared" si="0"/>
+        <v>38127</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>38163</v>
       </c>
@@ -1007,8 +1233,12 @@
       <c r="C56" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D56" s="1">
+        <f t="shared" si="0"/>
+        <v>38155</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>38197</v>
       </c>
@@ -1018,8 +1248,12 @@
       <c r="C57" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D57" s="1">
+        <f t="shared" si="0"/>
+        <v>38189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>38236</v>
       </c>
@@ -1029,8 +1263,12 @@
       <c r="C58" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D58" s="1">
+        <f t="shared" si="0"/>
+        <v>38228</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>38260</v>
       </c>
@@ -1040,8 +1278,12 @@
       <c r="C59" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D59" s="1">
+        <f t="shared" si="0"/>
+        <v>38252</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>38279</v>
       </c>
@@ -1051,8 +1293,12 @@
       <c r="C60" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D60" s="1">
+        <f t="shared" si="0"/>
+        <v>38271</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>38290</v>
       </c>
@@ -1062,8 +1308,12 @@
       <c r="C61" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D61" s="1">
+        <f t="shared" si="0"/>
+        <v>38282</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>38354</v>
       </c>
@@ -1073,8 +1323,12 @@
       <c r="C62" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D62" s="1">
+        <f t="shared" si="0"/>
+        <v>38346</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>38387</v>
       </c>
@@ -1084,8 +1338,12 @@
       <c r="C63" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D63" s="1">
+        <f t="shared" si="0"/>
+        <v>38379</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>38435</v>
       </c>
@@ -1095,8 +1353,12 @@
       <c r="C64" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D64" s="1">
+        <f t="shared" si="0"/>
+        <v>38427</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>38446</v>
       </c>
@@ -1106,8 +1368,12 @@
       <c r="C65" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D65" s="1">
+        <f t="shared" si="0"/>
+        <v>38438</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>38476</v>
       </c>
@@ -1117,8 +1383,12 @@
       <c r="C66" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D66" s="1">
+        <f t="shared" si="0"/>
+        <v>38468</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>38516</v>
       </c>
@@ -1128,8 +1398,12 @@
       <c r="C67" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D67" s="1">
+        <f t="shared" ref="D67:D130" si="1">A67-8</f>
+        <v>38508</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>38533</v>
       </c>
@@ -1139,8 +1413,12 @@
       <c r="C68" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D68" s="1">
+        <f t="shared" si="1"/>
+        <v>38525</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>38566</v>
       </c>
@@ -1150,8 +1428,12 @@
       <c r="C69" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D69" s="1">
+        <f t="shared" si="1"/>
+        <v>38558</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>38590</v>
       </c>
@@ -1161,8 +1443,12 @@
       <c r="C70" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D70" s="1">
+        <f t="shared" si="1"/>
+        <v>38582</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>38622</v>
       </c>
@@ -1172,8 +1458,12 @@
       <c r="C71" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D71" s="1">
+        <f t="shared" si="1"/>
+        <v>38614</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>38664</v>
       </c>
@@ -1183,8 +1473,12 @@
       <c r="C72" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D72" s="1">
+        <f t="shared" si="1"/>
+        <v>38656</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>38692</v>
       </c>
@@ -1194,8 +1488,12 @@
       <c r="C73" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D73" s="1">
+        <f t="shared" si="1"/>
+        <v>38684</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>38709</v>
       </c>
@@ -1205,8 +1503,12 @@
       <c r="C74" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D74" s="1">
+        <f t="shared" si="1"/>
+        <v>38701</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>38756</v>
       </c>
@@ -1216,8 +1518,12 @@
       <c r="C75" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D75" s="1">
+        <f t="shared" si="1"/>
+        <v>38748</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>38804</v>
       </c>
@@ -1227,8 +1533,12 @@
       <c r="C76" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D76" s="1">
+        <f t="shared" si="1"/>
+        <v>38796</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>38852</v>
       </c>
@@ -1238,8 +1548,12 @@
       <c r="C77" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D77" s="1">
+        <f t="shared" si="1"/>
+        <v>38844</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>38910</v>
       </c>
@@ -1249,8 +1563,12 @@
       <c r="C78" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D78" s="1">
+        <f t="shared" si="1"/>
+        <v>38902</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>38943</v>
       </c>
@@ -1260,8 +1578,12 @@
       <c r="C79" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D79" s="1">
+        <f t="shared" si="1"/>
+        <v>38935</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>38975</v>
       </c>
@@ -1271,8 +1593,12 @@
       <c r="C80" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D80" s="1">
+        <f t="shared" si="1"/>
+        <v>38967</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>39027</v>
       </c>
@@ -1282,8 +1608,12 @@
       <c r="C81" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D81" s="1">
+        <f t="shared" si="1"/>
+        <v>39019</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>39072</v>
       </c>
@@ -1293,8 +1623,12 @@
       <c r="C82" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D82" s="1">
+        <f t="shared" si="1"/>
+        <v>39064</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>39134</v>
       </c>
@@ -1304,8 +1638,12 @@
       <c r="C83" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D83" s="1">
+        <f t="shared" si="1"/>
+        <v>39126</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>39182</v>
       </c>
@@ -1315,8 +1653,12 @@
       <c r="C84" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D84" s="1">
+        <f t="shared" si="1"/>
+        <v>39174</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>39261</v>
       </c>
@@ -1326,8 +1668,12 @@
       <c r="C85" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D85" s="1">
+        <f t="shared" si="1"/>
+        <v>39253</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>39322</v>
       </c>
@@ -1337,8 +1683,12 @@
       <c r="C86" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D86" s="1">
+        <f t="shared" si="1"/>
+        <v>39314</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>39322</v>
       </c>
@@ -1348,8 +1698,12 @@
       <c r="C87" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D87" s="1">
+        <f t="shared" si="1"/>
+        <v>39314</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>39353</v>
       </c>
@@ -1359,8 +1713,12 @@
       <c r="C88" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D88" s="1">
+        <f t="shared" si="1"/>
+        <v>39345</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>39416</v>
       </c>
@@ -1370,8 +1728,12 @@
       <c r="C89" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D89" s="1">
+        <f t="shared" si="1"/>
+        <v>39408</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>39465</v>
       </c>
@@ -1381,8 +1743,12 @@
       <c r="C90" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D90" s="1">
+        <f t="shared" si="1"/>
+        <v>39457</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>39498</v>
       </c>
@@ -1392,8 +1758,12 @@
       <c r="C91" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D91" s="1">
+        <f t="shared" si="1"/>
+        <v>39490</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>39542</v>
       </c>
@@ -1403,8 +1773,12 @@
       <c r="C92" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D92" s="1">
+        <f t="shared" si="1"/>
+        <v>39534</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>39584</v>
       </c>
@@ -1414,8 +1788,12 @@
       <c r="C93" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D93" s="1">
+        <f t="shared" si="1"/>
+        <v>39576</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>39626</v>
       </c>
@@ -1425,8 +1803,12 @@
       <c r="C94" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D94" s="1">
+        <f t="shared" si="1"/>
+        <v>39618</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>39674</v>
       </c>
@@ -1436,8 +1818,12 @@
       <c r="C95" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D95" s="1">
+        <f t="shared" si="1"/>
+        <v>39666</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>39728</v>
       </c>
@@ -1447,8 +1833,12 @@
       <c r="C96" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D96" s="1">
+        <f t="shared" si="1"/>
+        <v>39720</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>39785</v>
       </c>
@@ -1458,8 +1848,12 @@
       <c r="C97" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D97" s="1">
+        <f t="shared" si="1"/>
+        <v>39777</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>39808</v>
       </c>
@@ -1469,8 +1863,12 @@
       <c r="C98" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D98" s="1">
+        <f t="shared" si="1"/>
+        <v>39800</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>39864</v>
       </c>
@@ -1480,8 +1878,12 @@
       <c r="C99" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D99" s="1">
+        <f t="shared" si="1"/>
+        <v>39856</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>39923</v>
       </c>
@@ -1491,8 +1893,12 @@
       <c r="C100" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D100" s="1">
+        <f t="shared" si="1"/>
+        <v>39915</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>39878</v>
       </c>
@@ -1502,8 +1908,12 @@
       <c r="C101" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D101" s="1">
+        <f t="shared" si="1"/>
+        <v>39870</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>40004</v>
       </c>
@@ -1513,8 +1923,12 @@
       <c r="C102" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D102" s="1">
+        <f t="shared" si="1"/>
+        <v>39996</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>40052</v>
       </c>
@@ -1524,8 +1938,12 @@
       <c r="C103" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D103" s="1">
+        <f t="shared" si="1"/>
+        <v>40044</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>40087</v>
       </c>
@@ -1535,8 +1953,12 @@
       <c r="C104" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D104" s="1">
+        <f t="shared" si="1"/>
+        <v>40079</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>40137</v>
       </c>
@@ -1546,8 +1968,12 @@
       <c r="C105" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D105" s="1">
+        <f t="shared" si="1"/>
+        <v>40129</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>40184</v>
       </c>
@@ -1557,8 +1983,12 @@
       <c r="C106" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D106" s="1">
+        <f t="shared" si="1"/>
+        <v>40176</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>40246</v>
       </c>
@@ -1568,8 +1998,12 @@
       <c r="C107" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D107" s="1">
+        <f t="shared" si="1"/>
+        <v>40238</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>40287</v>
       </c>
@@ -1579,8 +2013,12 @@
       <c r="C108" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D108" s="1">
+        <f t="shared" si="1"/>
+        <v>40279</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>40310</v>
       </c>
@@ -1590,8 +2028,12 @@
       <c r="C109" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D109" s="1">
+        <f t="shared" si="1"/>
+        <v>40302</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>40351</v>
       </c>
@@ -1601,8 +2043,12 @@
       <c r="C110" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D110" s="1">
+        <f t="shared" si="1"/>
+        <v>40343</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>40395</v>
       </c>
@@ -1612,8 +2058,12 @@
       <c r="C111" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D111" s="1">
+        <f t="shared" si="1"/>
+        <v>40387</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>40445</v>
       </c>
@@ -1623,8 +2073,12 @@
       <c r="C112" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D112" s="1">
+        <f t="shared" si="1"/>
+        <v>40437</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>40493</v>
       </c>
@@ -1634,8 +2088,12 @@
       <c r="C113" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D113" s="1">
+        <f t="shared" si="1"/>
+        <v>40485</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>40539</v>
       </c>
@@ -1645,8 +2103,12 @@
       <c r="C114" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D114" s="1">
+        <f t="shared" si="1"/>
+        <v>40531</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>40582</v>
       </c>
@@ -1656,8 +2118,12 @@
       <c r="C115" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D115" s="1">
+        <f t="shared" si="1"/>
+        <v>40574</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>40624</v>
       </c>
@@ -1667,8 +2133,12 @@
       <c r="C116" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D116" s="1">
+        <f t="shared" si="1"/>
+        <v>40616</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>40668</v>
       </c>
@@ -1678,8 +2148,12 @@
       <c r="C117" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D117" s="1">
+        <f t="shared" si="1"/>
+        <v>40660</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>40715</v>
       </c>
@@ -1689,8 +2163,12 @@
       <c r="C118" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D118" s="1">
+        <f t="shared" si="1"/>
+        <v>40707</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>40760</v>
       </c>
@@ -1700,8 +2178,12 @@
       <c r="C119" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D119" s="1">
+        <f t="shared" si="1"/>
+        <v>40752</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>40800</v>
       </c>
@@ -1711,8 +2193,12 @@
       <c r="C120" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D120" s="1">
+        <f t="shared" si="1"/>
+        <v>40792</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>40855</v>
       </c>
@@ -1722,8 +2208,12 @@
       <c r="C121" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D121" s="1">
+        <f t="shared" si="1"/>
+        <v>40847</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>40893</v>
       </c>
@@ -1733,8 +2223,12 @@
       <c r="C122" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D122" s="1">
+        <f t="shared" si="1"/>
+        <v>40885</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>40946</v>
       </c>
@@ -1744,8 +2238,12 @@
       <c r="C123" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D123" s="1">
+        <f t="shared" si="1"/>
+        <v>40938</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>40991</v>
       </c>
@@ -1755,8 +2253,12 @@
       <c r="C124" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D124" s="1">
+        <f t="shared" si="1"/>
+        <v>40983</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>41036</v>
       </c>
@@ -1766,8 +2268,12 @@
       <c r="C125" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D125" s="1">
+        <f t="shared" si="1"/>
+        <v>41028</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>41078</v>
       </c>
@@ -1777,8 +2283,12 @@
       <c r="C126" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D126" s="1">
+        <f t="shared" si="1"/>
+        <v>41070</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>41116</v>
       </c>
@@ -1788,8 +2298,12 @@
       <c r="C127" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D127" s="1">
+        <f t="shared" si="1"/>
+        <v>41108</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>41166</v>
       </c>
@@ -1799,8 +2313,12 @@
       <c r="C128" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D128" s="1">
+        <f t="shared" si="1"/>
+        <v>41158</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>41207</v>
       </c>
@@ -1810,8 +2328,12 @@
       <c r="C129" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D129" s="1">
+        <f t="shared" si="1"/>
+        <v>41199</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>41255</v>
       </c>
@@ -1821,8 +2343,12 @@
       <c r="C130" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D130" s="1">
+        <f t="shared" si="1"/>
+        <v>41247</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>41306</v>
       </c>
@@ -1832,8 +2358,12 @@
       <c r="C131" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D131" s="1">
+        <f t="shared" ref="D131:D194" si="2">A131-8</f>
+        <v>41298</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>41355</v>
       </c>
@@ -1843,8 +2373,12 @@
       <c r="C132" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D132" s="1">
+        <f t="shared" si="2"/>
+        <v>41347</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>41400</v>
       </c>
@@ -1854,8 +2388,12 @@
       <c r="C133" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D133" s="1">
+        <f t="shared" si="2"/>
+        <v>41392</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>41439</v>
       </c>
@@ -1865,8 +2403,12 @@
       <c r="C134" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D134" s="1">
+        <f t="shared" si="2"/>
+        <v>41431</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>41480</v>
       </c>
@@ -1876,8 +2418,12 @@
       <c r="C135" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D135" s="1">
+        <f t="shared" si="2"/>
+        <v>41472</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>41530</v>
       </c>
@@ -1887,8 +2433,12 @@
       <c r="C136" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D136" s="1">
+        <f t="shared" si="2"/>
+        <v>41522</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>41571</v>
       </c>
@@ -1898,8 +2448,12 @@
       <c r="C137" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D137" s="1">
+        <f t="shared" si="2"/>
+        <v>41563</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>41621</v>
       </c>
@@ -1909,8 +2463,12 @@
       <c r="C138" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D138" s="1">
+        <f t="shared" si="2"/>
+        <v>41613</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>41670</v>
       </c>
@@ -1920,8 +2478,12 @@
       <c r="C139" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D139" s="1">
+        <f t="shared" si="2"/>
+        <v>41662</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>41711</v>
       </c>
@@ -1931,8 +2493,12 @@
       <c r="C140" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D140" s="1">
+        <f t="shared" si="2"/>
+        <v>41703</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>41744</v>
       </c>
@@ -1942,8 +2508,12 @@
       <c r="C141" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D141" s="1">
+        <f t="shared" si="2"/>
+        <v>41736</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>41803</v>
       </c>
@@ -1953,8 +2523,12 @@
       <c r="C142" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D142" s="1">
+        <f t="shared" si="2"/>
+        <v>41795</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>41850</v>
       </c>
@@ -1964,8 +2538,12 @@
       <c r="C143" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D143" s="1">
+        <f t="shared" si="2"/>
+        <v>41842</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>41898</v>
       </c>
@@ -1975,8 +2553,12 @@
       <c r="C144" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D144" s="1">
+        <f t="shared" si="2"/>
+        <v>41890</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>41955</v>
       </c>
@@ -1986,8 +2568,12 @@
       <c r="C145" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D145" s="1">
+        <f t="shared" si="2"/>
+        <v>41947</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>41990</v>
       </c>
@@ -1997,8 +2583,12 @@
       <c r="C146" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D146" s="1">
+        <f t="shared" si="2"/>
+        <v>41982</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>42039</v>
       </c>
@@ -2008,8 +2598,12 @@
       <c r="C147" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D147" s="1">
+        <f t="shared" si="2"/>
+        <v>42031</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>42082</v>
       </c>
@@ -2019,8 +2613,12 @@
       <c r="C148" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D148" s="1">
+        <f t="shared" si="2"/>
+        <v>42074</v>
+      </c>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>42138</v>
       </c>
@@ -2030,8 +2628,12 @@
       <c r="C149" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D149" s="1">
+        <f t="shared" si="2"/>
+        <v>42130</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>42172</v>
       </c>
@@ -2041,8 +2643,12 @@
       <c r="C150" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D150" s="1">
+        <f t="shared" si="2"/>
+        <v>42164</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>42229</v>
       </c>
@@ -2052,8 +2658,12 @@
       <c r="C151" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D151" s="1">
+        <f t="shared" si="2"/>
+        <v>42221</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>42263</v>
       </c>
@@ -2063,8 +2673,12 @@
       <c r="C152" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D152" s="1">
+        <f t="shared" si="2"/>
+        <v>42255</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>42313</v>
       </c>
@@ -2074,8 +2688,12 @@
       <c r="C153" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D153" s="1">
+        <f t="shared" si="2"/>
+        <v>42305</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>42347</v>
       </c>
@@ -2085,8 +2703,12 @@
       <c r="C154" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D154" s="1">
+        <f t="shared" si="2"/>
+        <v>42339</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>42403</v>
       </c>
@@ -2096,8 +2718,12 @@
       <c r="C155" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155" s="1">
+        <f t="shared" si="2"/>
+        <v>42395</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>42447</v>
       </c>
@@ -2107,8 +2733,12 @@
       <c r="C156" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D156" s="1">
+        <f t="shared" si="2"/>
+        <v>42439</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>42501</v>
       </c>
@@ -2118,8 +2748,12 @@
       <c r="C157" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D157" s="1">
+        <f t="shared" si="2"/>
+        <v>42493</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>42542</v>
       </c>
@@ -2129,8 +2763,12 @@
       <c r="C158" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D158" s="1">
+        <f t="shared" si="2"/>
+        <v>42534</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>42583</v>
       </c>
@@ -2140,8 +2778,12 @@
       <c r="C159" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D159" s="1">
+        <f t="shared" si="2"/>
+        <v>42575</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>42619</v>
       </c>
@@ -2151,8 +2793,12 @@
       <c r="C160" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D160" s="1">
+        <f t="shared" si="2"/>
+        <v>42611</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>42668</v>
       </c>
@@ -2162,8 +2808,12 @@
       <c r="C161" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D161" s="1">
+        <f t="shared" si="2"/>
+        <v>42660</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>42710</v>
       </c>
@@ -2173,8 +2823,12 @@
       <c r="C162" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D162" s="1">
+        <f t="shared" si="2"/>
+        <v>42702</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>42752</v>
       </c>
@@ -2184,8 +2838,12 @@
       <c r="C163" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D163" s="1">
+        <f t="shared" si="2"/>
+        <v>42744</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>42796</v>
       </c>
@@ -2195,8 +2853,12 @@
       <c r="C164" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" s="1">
+        <f t="shared" si="2"/>
+        <v>42788</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>42843</v>
       </c>
@@ -2206,8 +2868,12 @@
       <c r="C165" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D165" s="1">
+        <f t="shared" si="2"/>
+        <v>42835</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>42892</v>
       </c>
@@ -2217,8 +2883,12 @@
       <c r="C166" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D166" s="1">
+        <f t="shared" si="2"/>
+        <v>42884</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>42948</v>
       </c>
@@ -2228,8 +2898,12 @@
       <c r="C167" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167" s="1">
+        <f t="shared" si="2"/>
+        <v>42940</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>42991</v>
       </c>
@@ -2239,8 +2913,12 @@
       <c r="C168" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D168" s="1">
+        <f t="shared" si="2"/>
+        <v>42983</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>43039</v>
       </c>
@@ -2250,8 +2928,12 @@
       <c r="C169" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D169" s="1">
+        <f t="shared" si="2"/>
+        <v>43031</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>43081</v>
       </c>
@@ -2261,8 +2943,12 @@
       <c r="C170" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D170" s="1">
+        <f t="shared" si="2"/>
+        <v>43073</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>43146</v>
       </c>
@@ -2272,8 +2958,12 @@
       <c r="C171" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D171" s="1">
+        <f t="shared" si="2"/>
+        <v>43138</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>43186</v>
       </c>
@@ -2283,8 +2973,12 @@
       <c r="C172" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D172" s="1">
+        <f t="shared" si="2"/>
+        <v>43178</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>43242</v>
       </c>
@@ -2294,8 +2988,12 @@
       <c r="C173" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D173" s="1">
+        <f t="shared" si="2"/>
+        <v>43234</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>43277</v>
       </c>
@@ -2305,8 +3003,12 @@
       <c r="C174" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D174" s="1">
+        <f t="shared" si="2"/>
+        <v>43269</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>43319</v>
       </c>
@@ -2316,8 +3018,12 @@
       <c r="C175" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D175" s="1">
+        <f t="shared" si="2"/>
+        <v>43311</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>43368</v>
       </c>
@@ -2327,8 +3033,12 @@
       <c r="C176" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176" s="1">
+        <f t="shared" si="2"/>
+        <v>43360</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>43410</v>
       </c>
@@ -2338,8 +3048,12 @@
       <c r="C177" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177" s="1">
+        <f t="shared" si="2"/>
+        <v>43402</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>43452</v>
       </c>
@@ -2349,8 +3063,12 @@
       <c r="C178" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178" s="1">
+        <f t="shared" si="2"/>
+        <v>43444</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>43508</v>
       </c>
@@ -2360,8 +3078,12 @@
       <c r="C179" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179" s="1">
+        <f t="shared" si="2"/>
+        <v>43500</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>43550</v>
       </c>
@@ -2371,8 +3093,12 @@
       <c r="C180" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180" s="1">
+        <f t="shared" si="2"/>
+        <v>43542</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>43599</v>
       </c>
@@ -2382,8 +3108,12 @@
       <c r="C181" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181" s="1">
+        <f t="shared" si="2"/>
+        <v>43591</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>43641</v>
       </c>
@@ -2393,8 +3123,12 @@
       <c r="C182" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182" s="1">
+        <f t="shared" si="2"/>
+        <v>43633</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>43683</v>
       </c>
@@ -2404,8 +3138,12 @@
       <c r="C183" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183" s="1">
+        <f t="shared" si="2"/>
+        <v>43675</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>43732</v>
       </c>
@@ -2415,8 +3153,12 @@
       <c r="C184" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184" s="1">
+        <f t="shared" si="2"/>
+        <v>43724</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>43774</v>
       </c>
@@ -2426,8 +3168,12 @@
       <c r="C185" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185" s="1">
+        <f t="shared" si="2"/>
+        <v>43766</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>43816</v>
       </c>
@@ -2437,8 +3183,12 @@
       <c r="C186" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D186" s="1">
+        <f t="shared" si="2"/>
+        <v>43808</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>43872</v>
       </c>
@@ -2448,8 +3198,12 @@
       <c r="C187" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D187" s="1">
+        <f t="shared" si="2"/>
+        <v>43864</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>43913</v>
       </c>
@@ -2459,8 +3213,12 @@
       <c r="C188" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D188" s="1">
+        <f t="shared" si="2"/>
+        <v>43905</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>43963</v>
       </c>
@@ -2470,8 +3228,12 @@
       <c r="C189" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D189" s="1">
+        <f t="shared" si="2"/>
+        <v>43955</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44005</v>
       </c>
@@ -2481,8 +3243,12 @@
       <c r="C190" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D190" s="1">
+        <f t="shared" si="2"/>
+        <v>43997</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44054</v>
       </c>
@@ -2492,8 +3258,12 @@
       <c r="C191" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D191" s="1">
+        <f t="shared" si="2"/>
+        <v>44046</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44096</v>
       </c>
@@ -2503,8 +3273,12 @@
       <c r="C192" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D192" s="1">
+        <f t="shared" si="2"/>
+        <v>44088</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44138</v>
       </c>
@@ -2514,8 +3288,12 @@
       <c r="C193" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D193" s="1">
+        <f t="shared" si="2"/>
+        <v>44130</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44180</v>
       </c>
@@ -2525,8 +3303,12 @@
       <c r="C194" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D194" s="1">
+        <f t="shared" si="2"/>
+        <v>44172</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44222</v>
       </c>
@@ -2536,8 +3318,12 @@
       <c r="C195" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D195" s="1">
+        <f t="shared" ref="D195:D210" si="3">A195-8</f>
+        <v>44214</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44278</v>
       </c>
@@ -2547,8 +3333,12 @@
       <c r="C196" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D196" s="1">
+        <f t="shared" si="3"/>
+        <v>44270</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44327</v>
       </c>
@@ -2558,8 +3348,12 @@
       <c r="C197" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D197" s="1">
+        <f t="shared" si="3"/>
+        <v>44319</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44378</v>
       </c>
@@ -2569,8 +3363,12 @@
       <c r="C198" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D198" s="1">
+        <f t="shared" si="3"/>
+        <v>44370</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44419</v>
       </c>
@@ -2580,8 +3378,12 @@
       <c r="C199" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D199" s="1">
+        <f t="shared" si="3"/>
+        <v>44411</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44467</v>
       </c>
@@ -2591,8 +3393,12 @@
       <c r="C200" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D200" s="1">
+        <f t="shared" si="3"/>
+        <v>44459</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44503</v>
       </c>
@@ -2602,8 +3408,12 @@
       <c r="C201" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D201" s="1">
+        <f t="shared" si="3"/>
+        <v>44495</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44544</v>
       </c>
@@ -2613,8 +3423,12 @@
       <c r="C202" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D202" s="1">
+        <f t="shared" si="3"/>
+        <v>44536</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44600</v>
       </c>
@@ -2624,8 +3438,12 @@
       <c r="C203" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D203" s="1">
+        <f t="shared" si="3"/>
+        <v>44592</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44642</v>
       </c>
@@ -2635,8 +3453,12 @@
       <c r="C204" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D204" s="1">
+        <f t="shared" si="3"/>
+        <v>44634</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44691</v>
       </c>
@@ -2646,8 +3468,12 @@
       <c r="C205" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D205" s="1">
+        <f t="shared" si="3"/>
+        <v>44683</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44733</v>
       </c>
@@ -2657,8 +3483,12 @@
       <c r="C206" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D206" s="1">
+        <f t="shared" si="3"/>
+        <v>44725</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44782</v>
       </c>
@@ -2668,8 +3498,12 @@
       <c r="C207" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D207" s="1">
+        <f t="shared" si="3"/>
+        <v>44774</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44831</v>
       </c>
@@ -2679,8 +3513,12 @@
       <c r="C208" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D208" s="1">
+        <f t="shared" si="3"/>
+        <v>44823</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44866</v>
       </c>
@@ -2690,8 +3528,12 @@
       <c r="C209" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D209" s="1">
+        <f t="shared" si="3"/>
+        <v>44858</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44908</v>
       </c>
@@ -2700,6 +3542,10 @@
       </c>
       <c r="C210" t="s">
         <v>7</v>
+      </c>
+      <c r="D210" s="1">
+        <f t="shared" si="3"/>
+        <v>44900</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new treated data
</commit_message>
<xml_diff>
--- a/data/minutes/copom_dates.xlsx
+++ b/data/minutes/copom_dates.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="224">
   <si>
     <t>date</t>
   </si>
@@ -680,6 +680,12 @@
   </si>
   <si>
     <t>selic</t>
+  </si>
+  <si>
+    <t>selic_surprise_d</t>
+  </si>
+  <si>
+    <t>selic_surprise_v</t>
   </si>
 </sst>
 </file>
@@ -715,9 +721,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1022,13 +1029,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H211"/>
+  <dimension ref="A1:J211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J8" sqref="J8"/>
+      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,10 +1046,11 @@
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1067,8 +1075,14 @@
       <c r="H1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="J1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>36558</v>
       </c>
@@ -1087,11 +1101,8 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>36579</v>
       </c>
@@ -1111,11 +1122,8 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="H3">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>36614</v>
       </c>
@@ -1134,11 +1142,8 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>36642</v>
       </c>
@@ -1157,11 +1162,8 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>36677</v>
       </c>
@@ -1180,11 +1182,8 @@
       <c r="F6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>36704</v>
       </c>
@@ -1203,11 +1202,8 @@
       <c r="F7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>36733</v>
       </c>
@@ -1226,11 +1222,8 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>36768</v>
       </c>
@@ -1249,11 +1242,8 @@
       <c r="F9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>36796</v>
       </c>
@@ -1272,11 +1262,8 @@
       <c r="F10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>36824</v>
       </c>
@@ -1295,11 +1282,8 @@
       <c r="F11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>36859</v>
       </c>
@@ -1318,11 +1302,8 @@
       <c r="F12">
         <v>0</v>
       </c>
-      <c r="H12">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>36887</v>
       </c>
@@ -1341,11 +1322,8 @@
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <v>15.75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>36915</v>
       </c>
@@ -1364,11 +1342,8 @@
       <c r="F14">
         <v>0</v>
       </c>
-      <c r="H14">
-        <v>15.25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>36949</v>
       </c>
@@ -1387,11 +1362,8 @@
       <c r="F15">
         <v>0</v>
       </c>
-      <c r="H15">
-        <v>15.25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>36978</v>
       </c>
@@ -1410,11 +1382,8 @@
       <c r="F16">
         <v>0</v>
       </c>
-      <c r="H16">
-        <v>15.75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>37006</v>
       </c>
@@ -1433,11 +1402,8 @@
       <c r="F17">
         <v>0</v>
       </c>
-      <c r="H17">
-        <v>16.25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>37041</v>
       </c>
@@ -1456,11 +1422,8 @@
       <c r="F18">
         <v>0</v>
       </c>
-      <c r="H18">
-        <v>16.75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>37069</v>
       </c>
@@ -1479,11 +1442,8 @@
       <c r="F19">
         <v>0</v>
       </c>
-      <c r="H19">
-        <v>18.25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>37097</v>
       </c>
@@ -1502,11 +1462,8 @@
       <c r="F20">
         <v>0</v>
       </c>
-      <c r="H20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>37132</v>
       </c>
@@ -1525,11 +1482,8 @@
       <c r="F21">
         <v>0</v>
       </c>
-      <c r="H21">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>37160</v>
       </c>
@@ -1548,11 +1502,8 @@
       <c r="F22">
         <v>0</v>
       </c>
-      <c r="H22">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>37188</v>
       </c>
@@ -1571,11 +1522,8 @@
       <c r="F23">
         <v>0</v>
       </c>
-      <c r="H23">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>37223</v>
       </c>
@@ -1594,11 +1542,8 @@
       <c r="F24">
         <v>0</v>
       </c>
-      <c r="H24">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>37251</v>
       </c>
@@ -1617,11 +1562,8 @@
       <c r="F25">
         <v>0</v>
       </c>
-      <c r="H25">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>37286</v>
       </c>
@@ -1640,11 +1582,8 @@
       <c r="F26">
         <v>0</v>
       </c>
-      <c r="H26">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>37314</v>
       </c>
@@ -1663,11 +1602,8 @@
       <c r="F27">
         <v>0</v>
       </c>
-      <c r="H27">
-        <v>18.75</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>37342</v>
       </c>
@@ -1686,11 +1622,8 @@
       <c r="F28">
         <v>0</v>
       </c>
-      <c r="H28">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>37370</v>
       </c>
@@ -1709,11 +1642,8 @@
       <c r="F29">
         <v>0</v>
       </c>
-      <c r="H29">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>37405</v>
       </c>
@@ -1732,11 +1662,8 @@
       <c r="F30">
         <v>0</v>
       </c>
-      <c r="H30">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>37433</v>
       </c>
@@ -1755,11 +1682,8 @@
       <c r="F31">
         <v>0</v>
       </c>
-      <c r="H31">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>37461</v>
       </c>
@@ -1778,11 +1702,8 @@
       <c r="F32">
         <v>0</v>
       </c>
-      <c r="H32">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>37496</v>
       </c>
@@ -1801,11 +1722,8 @@
       <c r="F33">
         <v>0</v>
       </c>
-      <c r="H33">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>37524</v>
       </c>
@@ -1824,11 +1742,8 @@
       <c r="F34">
         <v>0</v>
       </c>
-      <c r="H34">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>37545</v>
       </c>
@@ -1847,11 +1762,8 @@
       <c r="F35">
         <v>0</v>
       </c>
-      <c r="H35">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>37559</v>
       </c>
@@ -1870,11 +1782,8 @@
       <c r="F36">
         <v>0</v>
       </c>
-      <c r="H36">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>37587</v>
       </c>
@@ -1893,11 +1802,8 @@
       <c r="F37">
         <v>0</v>
       </c>
-      <c r="H37">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37614</v>
       </c>
@@ -1916,11 +1822,8 @@
       <c r="F38">
         <v>0</v>
       </c>
-      <c r="H38">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37650</v>
       </c>
@@ -1939,11 +1842,8 @@
       <c r="F39">
         <v>0</v>
       </c>
-      <c r="H39">
-        <v>25.5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>37678</v>
       </c>
@@ -1962,11 +1862,8 @@
       <c r="F40">
         <v>0</v>
       </c>
-      <c r="H40">
-        <v>26.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>37706</v>
       </c>
@@ -1985,11 +1882,8 @@
       <c r="F41">
         <v>0</v>
       </c>
-      <c r="H41">
-        <v>26.5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>37741</v>
       </c>
@@ -2008,11 +1902,8 @@
       <c r="F42">
         <v>0</v>
       </c>
-      <c r="H42">
-        <v>26.5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>37769</v>
       </c>
@@ -2031,11 +1922,8 @@
       <c r="F43">
         <v>0</v>
       </c>
-      <c r="H43">
-        <v>26.5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>37799</v>
       </c>
@@ -2054,11 +1942,8 @@
       <c r="F44">
         <v>0</v>
       </c>
-      <c r="H44">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>37833</v>
       </c>
@@ -2077,11 +1962,8 @@
       <c r="F45">
         <v>0</v>
       </c>
-      <c r="H45">
-        <v>24.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>37861</v>
       </c>
@@ -2100,11 +1982,8 @@
       <c r="F46">
         <v>0</v>
       </c>
-      <c r="H46">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>37888</v>
       </c>
@@ -2123,11 +2002,8 @@
       <c r="F47">
         <v>0</v>
       </c>
-      <c r="H47">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>37924</v>
       </c>
@@ -2146,11 +2022,8 @@
       <c r="F48">
         <v>0</v>
       </c>
-      <c r="H48">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>37952</v>
       </c>
@@ -2169,11 +2042,8 @@
       <c r="F49">
         <v>0</v>
       </c>
-      <c r="H49">
-        <v>17.5</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>37979</v>
       </c>
@@ -2192,11 +2062,8 @@
       <c r="F50">
         <v>0</v>
       </c>
-      <c r="H50">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>38033</v>
       </c>
@@ -2215,11 +2082,8 @@
       <c r="F51">
         <v>0</v>
       </c>
-      <c r="H51">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>38042</v>
       </c>
@@ -2238,11 +2102,8 @@
       <c r="F52">
         <v>0</v>
       </c>
-      <c r="H52">
-        <v>16.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>38071</v>
       </c>
@@ -2261,11 +2122,8 @@
       <c r="F53">
         <v>0</v>
       </c>
-      <c r="H53">
-        <v>16.25</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>38099</v>
       </c>
@@ -2284,11 +2142,8 @@
       <c r="F54">
         <v>0</v>
       </c>
-      <c r="H54">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>38134</v>
       </c>
@@ -2307,11 +2162,8 @@
       <c r="F55">
         <v>0</v>
       </c>
-      <c r="H55">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>38162</v>
       </c>
@@ -2330,11 +2182,8 @@
       <c r="F56">
         <v>0</v>
       </c>
-      <c r="H56">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>38197</v>
       </c>
@@ -2353,11 +2202,8 @@
       <c r="F57">
         <v>0</v>
       </c>
-      <c r="H57">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>38225</v>
       </c>
@@ -2376,11 +2222,8 @@
       <c r="F58">
         <v>0</v>
       </c>
-      <c r="H58">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>38253</v>
       </c>
@@ -2399,11 +2242,8 @@
       <c r="F59">
         <v>0</v>
       </c>
-      <c r="H59">
-        <v>16.25</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>38287</v>
       </c>
@@ -2422,11 +2262,8 @@
       <c r="F60">
         <v>0</v>
       </c>
-      <c r="H60">
-        <v>16.75</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>38316</v>
       </c>
@@ -2445,11 +2282,8 @@
       <c r="F61">
         <v>0</v>
       </c>
-      <c r="H61">
-        <v>17.25</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>38344</v>
       </c>
@@ -2469,11 +2303,8 @@
       <c r="F62">
         <v>0</v>
       </c>
-      <c r="H62">
-        <v>17.75</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>38379</v>
       </c>
@@ -2492,11 +2323,8 @@
       <c r="F63">
         <v>0</v>
       </c>
-      <c r="H63">
-        <v>18.25</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>38407</v>
       </c>
@@ -2515,11 +2343,8 @@
       <c r="F64">
         <v>0</v>
       </c>
-      <c r="H64">
-        <v>18.75</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>38435</v>
       </c>
@@ -2538,11 +2363,8 @@
       <c r="F65">
         <v>0</v>
       </c>
-      <c r="H65">
-        <v>19.25</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>38470</v>
       </c>
@@ -2561,11 +2383,8 @@
       <c r="F66">
         <v>0</v>
       </c>
-      <c r="H66">
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>38499</v>
       </c>
@@ -2584,11 +2403,8 @@
       <c r="F67">
         <v>0</v>
       </c>
-      <c r="H67">
-        <v>19.75</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>38526</v>
       </c>
@@ -2607,11 +2423,8 @@
       <c r="F68">
         <v>0</v>
       </c>
-      <c r="H68">
-        <v>19.75</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>38561</v>
       </c>
@@ -2630,11 +2443,8 @@
       <c r="F69">
         <v>0</v>
       </c>
-      <c r="H69">
-        <v>19.75</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>38589</v>
       </c>
@@ -2653,11 +2463,8 @@
       <c r="F70">
         <v>0</v>
       </c>
-      <c r="H70">
-        <v>19.75</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>38617</v>
       </c>
@@ -2676,11 +2483,8 @@
       <c r="F71">
         <v>0</v>
       </c>
-      <c r="H71">
-        <v>19.5</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>38652</v>
       </c>
@@ -2699,11 +2503,8 @@
       <c r="F72">
         <v>0</v>
       </c>
-      <c r="H72">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>38687</v>
       </c>
@@ -2722,11 +2523,8 @@
       <c r="F73">
         <v>0</v>
       </c>
-      <c r="H73">
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>38708</v>
       </c>
@@ -2745,11 +2543,8 @@
       <c r="F74">
         <v>0</v>
       </c>
-      <c r="H74">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>38743</v>
       </c>
@@ -2774,8 +2569,15 @@
       <c r="H75">
         <v>17.25</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="2">
+        <f t="shared" ref="I75:I130" si="1">H75-G75</f>
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>38792</v>
       </c>
@@ -2800,8 +2602,15 @@
       <c r="H76">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>38834</v>
       </c>
@@ -2826,8 +2635,15 @@
       <c r="H77">
         <v>15.75</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>38876</v>
       </c>
@@ -2852,8 +2668,15 @@
       <c r="H78">
         <v>15.25</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>38925</v>
       </c>
@@ -2878,8 +2701,15 @@
       <c r="H79">
         <v>14.75</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>38968</v>
       </c>
@@ -2904,8 +2734,16 @@
       <c r="H80">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.25</v>
+      </c>
+      <c r="J80">
+        <f t="shared" ref="J80:J139" si="2">IF(I80&lt;&gt;"0",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>39015</v>
       </c>
@@ -2930,8 +2768,15 @@
       <c r="H81">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>39058</v>
       </c>
@@ -2956,8 +2801,15 @@
       <c r="H82">
         <v>13.25</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>39114</v>
       </c>
@@ -2968,7 +2820,7 @@
         <v>4</v>
       </c>
       <c r="D83" s="1">
-        <f t="shared" ref="D83:D90" si="1">A83-8</f>
+        <f t="shared" ref="D83:D90" si="3">A83-8</f>
         <v>39106</v>
       </c>
       <c r="E83" t="s">
@@ -2983,8 +2835,16 @@
       <c r="H83">
         <v>13</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>39156</v>
       </c>
@@ -2995,7 +2855,7 @@
         <v>4</v>
       </c>
       <c r="D84" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39148</v>
       </c>
       <c r="E84" t="s">
@@ -3010,8 +2870,15 @@
       <c r="H84">
         <v>12.75</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>39198</v>
       </c>
@@ -3022,7 +2889,7 @@
         <v>4</v>
       </c>
       <c r="D85" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39190</v>
       </c>
       <c r="E85" t="s">
@@ -3037,8 +2904,15 @@
       <c r="H85">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>39247</v>
       </c>
@@ -3049,7 +2923,7 @@
         <v>4</v>
       </c>
       <c r="D86" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39239</v>
       </c>
       <c r="E86" t="s">
@@ -3064,8 +2938,15 @@
       <c r="H86">
         <v>12</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>39289</v>
       </c>
@@ -3076,7 +2957,7 @@
         <v>4</v>
       </c>
       <c r="D87" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39281</v>
       </c>
       <c r="E87" t="s">
@@ -3091,8 +2972,15 @@
       <c r="H87">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>39338</v>
       </c>
@@ -3103,7 +2991,7 @@
         <v>4</v>
       </c>
       <c r="D88" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39330</v>
       </c>
       <c r="E88" t="s">
@@ -3118,8 +3006,15 @@
       <c r="H88">
         <v>11.25</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>39380</v>
       </c>
@@ -3130,7 +3025,7 @@
         <v>4</v>
       </c>
       <c r="D89" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39372</v>
       </c>
       <c r="E89" t="s">
@@ -3145,8 +3040,16 @@
       <c r="H89">
         <v>11.25</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="J89">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>39429</v>
       </c>
@@ -3157,7 +3060,7 @@
         <v>4</v>
       </c>
       <c r="D90" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>39421</v>
       </c>
       <c r="E90" t="s">
@@ -3172,8 +3075,15 @@
       <c r="H90">
         <v>11.25</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>39478</v>
       </c>
@@ -3184,7 +3094,7 @@
         <v>4</v>
       </c>
       <c r="D91" s="1">
-        <f t="shared" ref="D91:D130" si="2">A91-8</f>
+        <f t="shared" ref="D91:D130" si="4">A91-8</f>
         <v>39470</v>
       </c>
       <c r="E91" t="s">
@@ -3199,8 +3109,15 @@
       <c r="H91">
         <v>11.25</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>39520</v>
       </c>
@@ -3211,7 +3128,7 @@
         <v>4</v>
       </c>
       <c r="D92" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39512</v>
       </c>
       <c r="E92" t="s">
@@ -3226,8 +3143,15 @@
       <c r="H92">
         <v>11.25</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>39562</v>
       </c>
@@ -3238,7 +3162,7 @@
         <v>4</v>
       </c>
       <c r="D93" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39554</v>
       </c>
       <c r="E93" t="s">
@@ -3253,8 +3177,16 @@
       <c r="H93">
         <v>11.75</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="J93">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>39611</v>
       </c>
@@ -3265,7 +3197,7 @@
         <v>4</v>
       </c>
       <c r="D94" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39603</v>
       </c>
       <c r="E94" t="s">
@@ -3280,8 +3212,15 @@
       <c r="H94">
         <v>12.25</v>
       </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I94" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>39660</v>
       </c>
@@ -3292,7 +3231,7 @@
         <v>4</v>
       </c>
       <c r="D95" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39652</v>
       </c>
       <c r="E95" t="s">
@@ -3307,8 +3246,16 @@
       <c r="H95">
         <v>13</v>
       </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I95" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="J95">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>39709</v>
       </c>
@@ -3319,7 +3266,7 @@
         <v>4</v>
       </c>
       <c r="D96" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39701</v>
       </c>
       <c r="E96" t="s">
@@ -3334,8 +3281,15 @@
       <c r="H96">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I96" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>39758</v>
       </c>
@@ -3346,7 +3300,7 @@
         <v>4</v>
       </c>
       <c r="D97" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39750</v>
       </c>
       <c r="E97" t="s">
@@ -3361,8 +3315,16 @@
       <c r="H97">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I97" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.5</v>
+      </c>
+      <c r="J97">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>39800</v>
       </c>
@@ -3373,7 +3335,7 @@
         <v>4</v>
       </c>
       <c r="D98" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39792</v>
       </c>
       <c r="E98" t="s">
@@ -3388,8 +3350,15 @@
       <c r="H98">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I98" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>39842</v>
       </c>
@@ -3400,7 +3369,7 @@
         <v>4</v>
       </c>
       <c r="D99" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39834</v>
       </c>
       <c r="E99" t="s">
@@ -3415,8 +3384,16 @@
       <c r="H99">
         <v>12.75</v>
       </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I99" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.38000000000000078</v>
+      </c>
+      <c r="J99">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>39891</v>
       </c>
@@ -3427,7 +3404,7 @@
         <v>4</v>
       </c>
       <c r="D100" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39883</v>
       </c>
       <c r="E100" t="s">
@@ -3442,8 +3419,16 @@
       <c r="H100">
         <v>11.25</v>
       </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I100" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.5</v>
+      </c>
+      <c r="J100">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>39940</v>
       </c>
@@ -3454,7 +3439,7 @@
         <v>4</v>
       </c>
       <c r="D101" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39932</v>
       </c>
       <c r="E101" t="s">
@@ -3469,8 +3454,15 @@
       <c r="H101">
         <v>10.25</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>39982</v>
       </c>
@@ -3481,7 +3473,7 @@
         <v>4</v>
       </c>
       <c r="D102" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>39974</v>
       </c>
       <c r="E102" t="s">
@@ -3496,8 +3488,16 @@
       <c r="H102">
         <v>9.25</v>
       </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I102" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.16999999999999993</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>40024</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>4</v>
       </c>
       <c r="D103" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40016</v>
       </c>
       <c r="E103" t="s">
@@ -3523,8 +3523,15 @@
       <c r="H103">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I103" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>40066</v>
       </c>
@@ -3535,7 +3542,7 @@
         <v>4</v>
       </c>
       <c r="D104" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40058</v>
       </c>
       <c r="E104" t="s">
@@ -3550,8 +3557,15 @@
       <c r="H104">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I104" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>40115</v>
       </c>
@@ -3562,7 +3576,7 @@
         <v>4</v>
       </c>
       <c r="D105" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40107</v>
       </c>
       <c r="E105" t="s">
@@ -3577,8 +3591,15 @@
       <c r="H105">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I105" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>40164</v>
       </c>
@@ -3589,7 +3610,7 @@
         <v>4</v>
       </c>
       <c r="D106" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40156</v>
       </c>
       <c r="E106" t="s">
@@ -3604,8 +3625,15 @@
       <c r="H106">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I106" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>40213</v>
       </c>
@@ -3616,7 +3644,7 @@
         <v>4</v>
       </c>
       <c r="D107" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40205</v>
       </c>
       <c r="E107" t="s">
@@ -3631,8 +3659,15 @@
       <c r="H107">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I107" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>40262</v>
       </c>
@@ -3643,7 +3678,7 @@
         <v>4</v>
       </c>
       <c r="D108" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40254</v>
       </c>
       <c r="E108" t="s">
@@ -3658,8 +3693,15 @@
       <c r="H108">
         <v>8.75</v>
       </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I108" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>40304</v>
       </c>
@@ -3670,7 +3712,7 @@
         <v>4</v>
       </c>
       <c r="D109" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40296</v>
       </c>
       <c r="E109" t="s">
@@ -3685,8 +3727,16 @@
       <c r="H109">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I109" s="2">
+        <f t="shared" si="1"/>
+        <v>0.25</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>40346</v>
       </c>
@@ -3697,7 +3747,7 @@
         <v>4</v>
       </c>
       <c r="D110" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40338</v>
       </c>
       <c r="E110" t="s">
@@ -3712,8 +3762,15 @@
       <c r="H110">
         <v>10.25</v>
       </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I110" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>40388</v>
       </c>
@@ -3724,7 +3781,7 @@
         <v>4</v>
       </c>
       <c r="D111" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40380</v>
       </c>
       <c r="E111" t="s">
@@ -3739,8 +3796,16 @@
       <c r="H111">
         <v>10.75</v>
       </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I111" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.25</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>40430</v>
       </c>
@@ -3751,7 +3816,7 @@
         <v>4</v>
       </c>
       <c r="D112" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40422</v>
       </c>
       <c r="E112" t="s">
@@ -3766,8 +3831,15 @@
       <c r="H112">
         <v>10.75</v>
       </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I112" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>40479</v>
       </c>
@@ -3778,7 +3850,7 @@
         <v>4</v>
       </c>
       <c r="D113" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40471</v>
       </c>
       <c r="E113" t="s">
@@ -3793,8 +3865,15 @@
       <c r="H113">
         <v>10.75</v>
       </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I113" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>40528</v>
       </c>
@@ -3805,7 +3884,7 @@
         <v>4</v>
       </c>
       <c r="D114" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40520</v>
       </c>
       <c r="E114" t="s">
@@ -3820,8 +3899,15 @@
       <c r="H114">
         <v>10.75</v>
       </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I114" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>40570</v>
       </c>
@@ -3832,7 +3918,7 @@
         <v>4</v>
       </c>
       <c r="D115" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40562</v>
       </c>
       <c r="E115" t="s">
@@ -3847,8 +3933,15 @@
       <c r="H115">
         <v>11.25</v>
       </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I115" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>40612</v>
       </c>
@@ -3859,7 +3952,7 @@
         <v>4</v>
       </c>
       <c r="D116" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40604</v>
       </c>
       <c r="E116" t="s">
@@ -3874,8 +3967,15 @@
       <c r="H116">
         <v>11.75</v>
       </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I116" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J116">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>40661</v>
       </c>
@@ -3886,7 +3986,7 @@
         <v>4</v>
       </c>
       <c r="D117" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40653</v>
       </c>
       <c r="E117" t="s">
@@ -3901,8 +4001,16 @@
       <c r="H117">
         <v>12</v>
       </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I117" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.25</v>
+      </c>
+      <c r="J117">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>40710</v>
       </c>
@@ -3913,7 +4021,7 @@
         <v>4</v>
       </c>
       <c r="D118" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40702</v>
       </c>
       <c r="E118" t="s">
@@ -3928,8 +4036,15 @@
       <c r="H118">
         <v>12.25</v>
       </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I118" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J118">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>40752</v>
       </c>
@@ -3940,7 +4055,7 @@
         <v>4</v>
       </c>
       <c r="D119" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40744</v>
       </c>
       <c r="E119" t="s">
@@ -3955,8 +4070,15 @@
       <c r="H119">
         <v>12.5</v>
       </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I119" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J119">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>40794</v>
       </c>
@@ -3967,7 +4089,7 @@
         <v>4</v>
       </c>
       <c r="D120" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40786</v>
       </c>
       <c r="E120" t="s">
@@ -3982,8 +4104,16 @@
       <c r="H120">
         <v>12</v>
       </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I120" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.5</v>
+      </c>
+      <c r="J120">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>40843</v>
       </c>
@@ -3994,7 +4124,7 @@
         <v>4</v>
       </c>
       <c r="D121" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40835</v>
       </c>
       <c r="E121" t="s">
@@ -4009,8 +4139,15 @@
       <c r="H121">
         <v>11.5</v>
       </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I121" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J121">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>40885</v>
       </c>
@@ -4021,7 +4158,7 @@
         <v>4</v>
       </c>
       <c r="D122" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40877</v>
       </c>
       <c r="E122" t="s">
@@ -4036,8 +4173,15 @@
       <c r="H122">
         <v>11</v>
       </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I122" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>40934</v>
       </c>
@@ -4048,7 +4192,7 @@
         <v>5</v>
       </c>
       <c r="D123" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40926</v>
       </c>
       <c r="E123" t="s">
@@ -4063,8 +4207,15 @@
       <c r="H123">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I123" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J123">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>40983</v>
       </c>
@@ -4075,7 +4226,7 @@
         <v>5</v>
       </c>
       <c r="D124" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>40975</v>
       </c>
       <c r="E124" t="s">
@@ -4090,8 +4241,16 @@
       <c r="H124">
         <v>9.75</v>
       </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I124" s="2">
+        <f t="shared" si="1"/>
+        <v>-0.25</v>
+      </c>
+      <c r="J124">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>41025</v>
       </c>
@@ -4102,7 +4261,7 @@
         <v>5</v>
       </c>
       <c r="D125" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>41017</v>
       </c>
       <c r="E125" t="s">
@@ -4117,8 +4276,15 @@
       <c r="H125">
         <v>9</v>
       </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I125" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J125">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>41068</v>
       </c>
@@ -4129,7 +4295,7 @@
         <v>5</v>
       </c>
       <c r="D126" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>41060</v>
       </c>
       <c r="E126" t="s">
@@ -4144,8 +4310,15 @@
       <c r="H126">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I126" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J126">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>41109</v>
       </c>
@@ -4156,7 +4329,7 @@
         <v>5</v>
       </c>
       <c r="D127" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>41101</v>
       </c>
       <c r="E127" t="s">
@@ -4171,8 +4344,15 @@
       <c r="H127">
         <v>8</v>
       </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I127" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J127">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>41158</v>
       </c>
@@ -4183,7 +4363,7 @@
         <v>5</v>
       </c>
       <c r="D128" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>41150</v>
       </c>
       <c r="E128" t="s">
@@ -4198,8 +4378,15 @@
       <c r="H128">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I128" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J128">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>41200</v>
       </c>
@@ -4210,7 +4397,7 @@
         <v>5</v>
       </c>
       <c r="D129" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>41192</v>
       </c>
       <c r="E129" t="s">
@@ -4225,8 +4412,15 @@
       <c r="H129">
         <v>7.25</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I129" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J129">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>41249</v>
       </c>
@@ -4237,7 +4431,7 @@
         <v>5</v>
       </c>
       <c r="D130" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>41241</v>
       </c>
       <c r="E130" t="s">
@@ -4252,8 +4446,15 @@
       <c r="H130">
         <v>7.25</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I130" s="2">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J130">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>41298</v>
       </c>
@@ -4264,7 +4465,7 @@
         <v>5</v>
       </c>
       <c r="D131" s="1">
-        <f t="shared" ref="D131:D154" si="3">A131-8</f>
+        <f t="shared" ref="D131:D154" si="5">A131-8</f>
         <v>41290</v>
       </c>
       <c r="E131" t="s">
@@ -4279,8 +4480,15 @@
       <c r="H131">
         <v>7.25</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I131" s="2">
+        <f t="shared" ref="I131:I194" si="6">H131-G131</f>
+        <v>0</v>
+      </c>
+      <c r="J131">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>41347</v>
       </c>
@@ -4291,7 +4499,7 @@
         <v>5</v>
       </c>
       <c r="D132" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41339</v>
       </c>
       <c r="E132" t="s">
@@ -4306,8 +4514,15 @@
       <c r="H132">
         <v>7.25</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I132" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J132">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>41389</v>
       </c>
@@ -4318,7 +4533,7 @@
         <v>5</v>
       </c>
       <c r="D133" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41381</v>
       </c>
       <c r="E133" t="s">
@@ -4333,8 +4548,15 @@
       <c r="H133">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I133" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J133">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>41431</v>
       </c>
@@ -4345,7 +4567,7 @@
         <v>5</v>
       </c>
       <c r="D134" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41423</v>
       </c>
       <c r="E134" t="s">
@@ -4360,8 +4582,16 @@
       <c r="H134">
         <v>8</v>
       </c>
-    </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I134" s="2">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="J134">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>41473</v>
       </c>
@@ -4372,7 +4602,7 @@
         <v>5</v>
       </c>
       <c r="D135" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41465</v>
       </c>
       <c r="E135" t="s">
@@ -4387,8 +4617,15 @@
       <c r="H135">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I135" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J135">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>41522</v>
       </c>
@@ -4399,7 +4636,7 @@
         <v>5</v>
       </c>
       <c r="D136" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41514</v>
       </c>
       <c r="E136" t="s">
@@ -4414,8 +4651,15 @@
       <c r="H136">
         <v>9</v>
       </c>
-    </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I136" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J136">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>41564</v>
       </c>
@@ -4426,7 +4670,7 @@
         <v>5</v>
       </c>
       <c r="D137" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41556</v>
       </c>
       <c r="E137" t="s">
@@ -4441,8 +4685,15 @@
       <c r="H137">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I137" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J137">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>41613</v>
       </c>
@@ -4453,7 +4704,7 @@
         <v>5</v>
       </c>
       <c r="D138" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41605</v>
       </c>
       <c r="E138" t="s">
@@ -4468,8 +4719,15 @@
       <c r="H138">
         <v>10</v>
       </c>
-    </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I138" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J138">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>41662</v>
       </c>
@@ -4480,7 +4738,7 @@
         <v>5</v>
       </c>
       <c r="D139" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41654</v>
       </c>
       <c r="E139" t="s">
@@ -4495,8 +4753,16 @@
       <c r="H139">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I139" s="2">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="J139">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>41704</v>
       </c>
@@ -4507,7 +4773,7 @@
         <v>5</v>
       </c>
       <c r="D140" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41696</v>
       </c>
       <c r="E140" t="s">
@@ -4522,8 +4788,16 @@
       <c r="H140">
         <v>10.75</v>
       </c>
-    </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I140" s="2">
+        <f t="shared" si="6"/>
+        <v>-0.25</v>
+      </c>
+      <c r="J140">
+        <f t="shared" ref="J140:J201" si="7">IF(I140&lt;&gt;"0",1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>41739</v>
       </c>
@@ -4534,7 +4808,7 @@
         <v>5</v>
       </c>
       <c r="D141" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41731</v>
       </c>
       <c r="E141" t="s">
@@ -4549,8 +4823,15 @@
       <c r="H141">
         <v>11</v>
       </c>
-    </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I141" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J141">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>41795</v>
       </c>
@@ -4561,7 +4842,7 @@
         <v>5</v>
       </c>
       <c r="D142" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41787</v>
       </c>
       <c r="E142" t="s">
@@ -4576,8 +4857,15 @@
       <c r="H142">
         <v>11</v>
       </c>
-    </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I142" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>41844</v>
       </c>
@@ -4588,7 +4876,7 @@
         <v>5</v>
       </c>
       <c r="D143" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41836</v>
       </c>
       <c r="E143" t="s">
@@ -4603,8 +4891,15 @@
       <c r="H143">
         <v>11</v>
       </c>
-    </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I143" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>41893</v>
       </c>
@@ -4615,7 +4910,7 @@
         <v>5</v>
       </c>
       <c r="D144" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41885</v>
       </c>
       <c r="E144" t="s">
@@ -4630,8 +4925,15 @@
       <c r="H144">
         <v>11</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I144" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>41949</v>
       </c>
@@ -4642,7 +4944,7 @@
         <v>5</v>
       </c>
       <c r="D145" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41941</v>
       </c>
       <c r="E145" t="s">
@@ -4657,8 +4959,16 @@
       <c r="H145">
         <v>11.25</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I145" s="2">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="J145">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>41984</v>
       </c>
@@ -4669,7 +4979,7 @@
         <v>5</v>
       </c>
       <c r="D146" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>41976</v>
       </c>
       <c r="E146" t="s">
@@ -4684,8 +4994,15 @@
       <c r="H146">
         <v>11.75</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I146" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>42033</v>
       </c>
@@ -4696,7 +5013,7 @@
         <v>5</v>
       </c>
       <c r="D147" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42025</v>
       </c>
       <c r="E147" t="s">
@@ -4711,8 +5028,15 @@
       <c r="H147">
         <v>12.25</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I147" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>42075</v>
       </c>
@@ -4723,7 +5047,7 @@
         <v>5</v>
       </c>
       <c r="D148" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42067</v>
       </c>
       <c r="E148" t="s">
@@ -4738,8 +5062,15 @@
       <c r="H148">
         <v>12.75</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I148" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>42131</v>
       </c>
@@ -4750,7 +5081,7 @@
         <v>5</v>
       </c>
       <c r="D149" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42123</v>
       </c>
       <c r="E149" t="s">
@@ -4765,8 +5096,15 @@
       <c r="H149">
         <v>13.25</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I149" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>42166</v>
       </c>
@@ -4777,7 +5115,7 @@
         <v>5</v>
       </c>
       <c r="D150" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42158</v>
       </c>
       <c r="E150" t="s">
@@ -4792,8 +5130,15 @@
       <c r="H150">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I150" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>42222</v>
       </c>
@@ -4804,7 +5149,7 @@
         <v>5</v>
       </c>
       <c r="D151" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42214</v>
       </c>
       <c r="E151" t="s">
@@ -4819,8 +5164,15 @@
       <c r="H151">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I151" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>42257</v>
       </c>
@@ -4831,7 +5183,7 @@
         <v>5</v>
       </c>
       <c r="D152" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42249</v>
       </c>
       <c r="E152" t="s">
@@ -4846,8 +5198,15 @@
       <c r="H152">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I152" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>42306</v>
       </c>
@@ -4858,7 +5217,7 @@
         <v>5</v>
       </c>
       <c r="D153" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42298</v>
       </c>
       <c r="E153" t="s">
@@ -4873,8 +5232,15 @@
       <c r="H153">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I153" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>42341</v>
       </c>
@@ -4885,7 +5251,7 @@
         <v>5</v>
       </c>
       <c r="D154" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>42333</v>
       </c>
       <c r="E154" t="s">
@@ -4900,8 +5266,15 @@
       <c r="H154">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I154" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>42397</v>
       </c>
@@ -4926,8 +5299,16 @@
       <c r="H155">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I155" s="2">
+        <f t="shared" si="6"/>
+        <v>-0.5</v>
+      </c>
+      <c r="J155">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>42439</v>
       </c>
@@ -4952,8 +5333,15 @@
       <c r="H156">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I156" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>42495</v>
       </c>
@@ -4978,8 +5366,15 @@
       <c r="H157">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I157" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>42537</v>
       </c>
@@ -5004,8 +5399,15 @@
       <c r="H158">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I158" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>42577</v>
       </c>
@@ -5030,8 +5432,15 @@
       <c r="H159">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I159" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>42619</v>
       </c>
@@ -5056,8 +5465,15 @@
       <c r="H160">
         <v>14.25</v>
       </c>
-    </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I160" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>42668</v>
       </c>
@@ -5082,8 +5498,15 @@
       <c r="H161">
         <v>14</v>
       </c>
-    </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I161" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>42710</v>
       </c>
@@ -5108,8 +5531,15 @@
       <c r="H162">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I162" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>42752</v>
       </c>
@@ -5134,8 +5564,16 @@
       <c r="H163">
         <v>13</v>
       </c>
-    </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I163" s="2">
+        <f t="shared" si="6"/>
+        <v>-0.25</v>
+      </c>
+      <c r="J163">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>42796</v>
       </c>
@@ -5160,8 +5598,15 @@
       <c r="H164">
         <v>12.25</v>
       </c>
-    </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I164" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>42843</v>
       </c>
@@ -5186,8 +5631,15 @@
       <c r="H165">
         <v>11.25</v>
       </c>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I165" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>42892</v>
       </c>
@@ -5212,8 +5664,15 @@
       <c r="H166">
         <v>10.25</v>
       </c>
-    </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I166" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J166">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>42948</v>
       </c>
@@ -5238,8 +5697,15 @@
       <c r="H167">
         <v>9.25</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I167" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J167">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>42990</v>
       </c>
@@ -5264,8 +5730,15 @@
       <c r="H168">
         <v>8.25</v>
       </c>
-    </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I168" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J168">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="169" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>43039</v>
       </c>
@@ -5290,8 +5763,15 @@
       <c r="H169">
         <v>7.5</v>
       </c>
-    </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I169" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J169">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>43081</v>
       </c>
@@ -5316,8 +5796,15 @@
       <c r="H170">
         <v>7</v>
       </c>
-    </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I170" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J170">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>43146</v>
       </c>
@@ -5342,8 +5829,15 @@
       <c r="H171">
         <v>6.75</v>
       </c>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I171" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J171">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="172" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>43186</v>
       </c>
@@ -5368,8 +5862,15 @@
       <c r="H172">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I172" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J172">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>43242</v>
       </c>
@@ -5394,8 +5895,16 @@
       <c r="H173">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I173" s="2">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+      <c r="J173">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>43277</v>
       </c>
@@ -5420,8 +5929,15 @@
       <c r="H174">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I174" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J174">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>43319</v>
       </c>
@@ -5446,8 +5962,15 @@
       <c r="H175">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I175" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J175">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>43368</v>
       </c>
@@ -5472,8 +5995,15 @@
       <c r="H176">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I176" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J176">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>43410</v>
       </c>
@@ -5498,8 +6028,15 @@
       <c r="H177">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I177" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J177">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>43452</v>
       </c>
@@ -5524,8 +6061,15 @@
       <c r="H178">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I178" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J178">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>43508</v>
       </c>
@@ -5550,8 +6094,15 @@
       <c r="H179">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I179" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J179">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>43550</v>
       </c>
@@ -5576,8 +6127,15 @@
       <c r="H180">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I180" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J180">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>43599</v>
       </c>
@@ -5602,8 +6160,15 @@
       <c r="H181">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I181" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>43641</v>
       </c>
@@ -5628,8 +6193,15 @@
       <c r="H182">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I182" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J182">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="183" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>43683</v>
       </c>
@@ -5654,8 +6226,16 @@
       <c r="H183">
         <v>6</v>
       </c>
-    </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I183" s="2">
+        <f t="shared" si="6"/>
+        <v>-5.9999999999999609E-2</v>
+      </c>
+      <c r="J183">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>43732</v>
       </c>
@@ -5680,8 +6260,15 @@
       <c r="H184">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I184" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J184">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="185" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>43774</v>
       </c>
@@ -5706,8 +6293,15 @@
       <c r="H185">
         <v>5</v>
       </c>
-    </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I185" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>43816</v>
       </c>
@@ -5732,8 +6326,15 @@
       <c r="H186">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I186" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>43872</v>
       </c>
@@ -5758,8 +6359,15 @@
       <c r="H187">
         <v>4.25</v>
       </c>
-    </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I187" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>43913</v>
       </c>
@@ -5784,8 +6392,16 @@
       <c r="H188">
         <v>3.75</v>
       </c>
-    </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I188" s="2">
+        <f t="shared" si="6"/>
+        <v>-0.25</v>
+      </c>
+      <c r="J188">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>43963</v>
       </c>
@@ -5810,8 +6426,16 @@
       <c r="H189">
         <v>3</v>
       </c>
-    </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I189" s="2">
+        <f t="shared" si="6"/>
+        <v>-0.25</v>
+      </c>
+      <c r="J189">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>44005</v>
       </c>
@@ -5836,8 +6460,15 @@
       <c r="H190">
         <v>2.25</v>
       </c>
-    </row>
-    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I190" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J190">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>44054</v>
       </c>
@@ -5862,8 +6493,15 @@
       <c r="H191">
         <v>2</v>
       </c>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I191" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J191">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>44096</v>
       </c>
@@ -5888,8 +6526,15 @@
       <c r="H192">
         <v>2</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I192" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J192">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>44138</v>
       </c>
@@ -5914,8 +6559,15 @@
       <c r="H193">
         <v>2</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I193" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J193">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="194" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>44180</v>
       </c>
@@ -5940,8 +6592,15 @@
       <c r="H194">
         <v>2</v>
       </c>
-    </row>
-    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I194" s="2">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J194">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="195" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>44222</v>
       </c>
@@ -5966,8 +6625,15 @@
       <c r="H195">
         <v>2</v>
       </c>
-    </row>
-    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I195" s="2">
+        <f t="shared" ref="I195:I210" si="8">H195-G195</f>
+        <v>0</v>
+      </c>
+      <c r="J195">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>44278</v>
       </c>
@@ -5992,8 +6658,16 @@
       <c r="H196">
         <v>2.75</v>
       </c>
-    </row>
-    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I196" s="2">
+        <f t="shared" si="8"/>
+        <v>0.25</v>
+      </c>
+      <c r="J196">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>44327</v>
       </c>
@@ -6018,8 +6692,15 @@
       <c r="H197">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I197" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J197">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>44369</v>
       </c>
@@ -6044,8 +6725,15 @@
       <c r="H198">
         <v>4.25</v>
       </c>
-    </row>
-    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I198" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J198">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="199" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>44418</v>
       </c>
@@ -6070,8 +6758,15 @@
       <c r="H199">
         <v>5.25</v>
       </c>
-    </row>
-    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I199" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>44467</v>
       </c>
@@ -6096,8 +6791,15 @@
       <c r="H200">
         <v>6.25</v>
       </c>
-    </row>
-    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I200" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>44503</v>
       </c>
@@ -6122,8 +6824,16 @@
       <c r="H201">
         <v>7.75</v>
       </c>
-    </row>
-    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I201" s="2">
+        <f t="shared" si="8"/>
+        <v>0.125</v>
+      </c>
+      <c r="J201">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="202" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>44544</v>
       </c>
@@ -6148,8 +6858,15 @@
       <c r="H202">
         <v>9.25</v>
       </c>
-    </row>
-    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I202" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J202">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="203" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>44600</v>
       </c>
@@ -6174,8 +6891,15 @@
       <c r="H203">
         <v>10.75</v>
       </c>
-    </row>
-    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I203" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J203">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="204" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>44644</v>
       </c>
@@ -6200,8 +6924,15 @@
       <c r="H204">
         <v>11.75</v>
       </c>
-    </row>
-    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I204" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>44691</v>
       </c>
@@ -6226,8 +6957,15 @@
       <c r="H205">
         <v>12.75</v>
       </c>
-    </row>
-    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I205" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>44733</v>
       </c>
@@ -6252,8 +6990,15 @@
       <c r="H206">
         <v>13.25</v>
       </c>
-    </row>
-    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I206" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>44782</v>
       </c>
@@ -6278,8 +7023,15 @@
       <c r="H207">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I207" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>44831</v>
       </c>
@@ -6304,8 +7056,15 @@
       <c r="H208">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I208" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>44866</v>
       </c>
@@ -6330,8 +7089,15 @@
       <c r="H209">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I209" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J209">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>44908</v>
       </c>
@@ -6356,8 +7122,15 @@
       <c r="H210">
         <v>13.75</v>
       </c>
-    </row>
-    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I210" s="2">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="J210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D211" s="1"/>
     </row>
   </sheetData>

</xml_diff>